<commit_message>
Completing the rest of the excel sheet for the Sydeny - Melbourne Railway Line.
</commit_message>
<xml_diff>
--- a/data/Processed_Data/Stations.xlsx
+++ b/data/Processed_Data/Stations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Academic\Aus_Trains\data\Processed_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59981073-C7F0-4929-89B5-50B83EB0A58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E418FF3A-B702-4D68-91C9-FB326EDD46A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3AE5864F-F506-40FE-BEF5-325CAB23D357}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="75">
   <si>
     <t>Station_ID</t>
   </si>
@@ -176,12 +176,6 @@
     <t>VIC</t>
   </si>
   <si>
-    <t>MelbourneMetro</t>
-  </si>
-  <si>
-    <t>NorthernMetro</t>
-  </si>
-  <si>
     <t>Hume</t>
   </si>
   <si>
@@ -243,6 +237,30 @@
   </si>
   <si>
     <t>-36.0760</t>
+  </si>
+  <si>
+    <t>Northern Victoria</t>
+  </si>
+  <si>
+    <t>MelbourneMetropolitan</t>
+  </si>
+  <si>
+    <t>Northern Metropolitan</t>
+  </si>
+  <si>
+    <t>-37.8183</t>
+  </si>
+  <si>
+    <t>-37.6806</t>
+  </si>
+  <si>
+    <t>-37.0264</t>
+  </si>
+  <si>
+    <t>-36.5515</t>
+  </si>
+  <si>
+    <t>-36.3573</t>
   </si>
 </sst>
 </file>
@@ -623,15 +641,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A3C533-154F-42EF-A106-DD2085AC4224}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="25.109375" customWidth="1"/>
     <col min="3" max="3" width="10.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
   </cols>
@@ -667,10 +685,10 @@
         <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F4">
         <v>151.20500000000001</v>
@@ -687,10 +705,10 @@
         <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F5">
         <v>150.81399999999999</v>
@@ -707,10 +725,10 @@
         <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F6">
         <v>150.375</v>
@@ -727,10 +745,10 @@
         <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F7">
         <v>149.7209</v>
@@ -747,10 +765,10 @@
         <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F8">
         <v>149.26499999999999</v>
@@ -767,10 +785,10 @@
         <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F9">
         <v>148.911</v>
@@ -787,10 +805,10 @@
         <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F10">
         <v>148.38</v>
@@ -807,10 +825,10 @@
         <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F11">
         <v>148.02799999999999</v>
@@ -827,10 +845,10 @@
         <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F12">
         <v>147.58699999999999</v>
@@ -847,10 +865,10 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F13">
         <v>147.37</v>
@@ -867,10 +885,10 @@
         <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F14">
         <v>147.15199999999999</v>
@@ -887,10 +905,10 @@
         <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F15">
         <v>147.036</v>
@@ -907,10 +925,10 @@
         <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F16">
         <v>146.94999999999999</v>
@@ -927,10 +945,10 @@
         <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F17">
         <v>146.91999999999999</v>
@@ -947,7 +965,13 @@
         <v>45</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>68</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22">
+        <v>144.95249999999999</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -961,7 +985,13 @@
         <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>69</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23">
+        <v>144.91829999999999</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -975,7 +1005,13 @@
         <v>45</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>67</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24">
+        <v>145.1344</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -989,7 +1025,13 @@
         <v>45</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25">
+        <v>145.9836</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1003,7 +1045,13 @@
         <v>45</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26">
+        <v>146.3252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completing another two railway line. Two more to go
</commit_message>
<xml_diff>
--- a/data/Processed_Data/Stations.xlsx
+++ b/data/Processed_Data/Stations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Academic\Aus_Trains\data\Processed_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E418FF3A-B702-4D68-91C9-FB326EDD46A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5947955E-5280-4446-B058-6F80A4B538FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3AE5864F-F506-40FE-BEF5-325CAB23D357}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="157">
   <si>
     <t>Station_ID</t>
   </si>
@@ -261,6 +261,252 @@
   </si>
   <si>
     <t>-36.3573</t>
+  </si>
+  <si>
+    <t>North Shore</t>
+  </si>
+  <si>
+    <t>Arrarat</t>
+  </si>
+  <si>
+    <t>Stawell</t>
+  </si>
+  <si>
+    <t>Horsham</t>
+  </si>
+  <si>
+    <t>Dimboola</t>
+  </si>
+  <si>
+    <t>Nhill</t>
+  </si>
+  <si>
+    <t>VIC_06</t>
+  </si>
+  <si>
+    <t>VIC_07</t>
+  </si>
+  <si>
+    <t>VIC_08</t>
+  </si>
+  <si>
+    <t>VIC_09</t>
+  </si>
+  <si>
+    <t>VIC_10</t>
+  </si>
+  <si>
+    <t>VIC_11</t>
+  </si>
+  <si>
+    <t>SA_01</t>
+  </si>
+  <si>
+    <t>SA_02</t>
+  </si>
+  <si>
+    <t>Adelaide Parklands</t>
+  </si>
+  <si>
+    <t>Murray Bridge</t>
+  </si>
+  <si>
+    <t>Bordertown</t>
+  </si>
+  <si>
+    <t>SA_03</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>Wimmera</t>
+  </si>
+  <si>
+    <t>Greater Geelong</t>
+  </si>
+  <si>
+    <t>Grampians</t>
+  </si>
+  <si>
+    <t>-38.0830</t>
+  </si>
+  <si>
+    <t>-37.2865</t>
+  </si>
+  <si>
+    <t>-37.0564</t>
+  </si>
+  <si>
+    <t>-36.7114</t>
+  </si>
+  <si>
+    <t>-36.4544</t>
+  </si>
+  <si>
+    <t>-36.3330</t>
+  </si>
+  <si>
+    <t>Limestone Coast</t>
+  </si>
+  <si>
+    <t>Murray Lands &amp; Riverlands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adelaide Metro </t>
+  </si>
+  <si>
+    <t>-34.9450</t>
+  </si>
+  <si>
+    <t>-35.1190</t>
+  </si>
+  <si>
+    <t>-36.3120</t>
+  </si>
+  <si>
+    <t>Strathfield Station</t>
+  </si>
+  <si>
+    <t>Paramatta Station</t>
+  </si>
+  <si>
+    <t>Penrith Station</t>
+  </si>
+  <si>
+    <t>Katoomba Station</t>
+  </si>
+  <si>
+    <t>Lithgow Station</t>
+  </si>
+  <si>
+    <t>Bathurst Staion</t>
+  </si>
+  <si>
+    <t>Blayney Station</t>
+  </si>
+  <si>
+    <t>Orange Station</t>
+  </si>
+  <si>
+    <t>Parkes Station</t>
+  </si>
+  <si>
+    <t>Condobolin Station</t>
+  </si>
+  <si>
+    <t>Eubalong West Station</t>
+  </si>
+  <si>
+    <t>Ivanhoe Station</t>
+  </si>
+  <si>
+    <t>Darnick Station</t>
+  </si>
+  <si>
+    <t>Menindee Station</t>
+  </si>
+  <si>
+    <t>Broken Hill</t>
+  </si>
+  <si>
+    <t>NSW_15</t>
+  </si>
+  <si>
+    <t>NSW_16</t>
+  </si>
+  <si>
+    <t>NSW_17</t>
+  </si>
+  <si>
+    <t>NSW_18</t>
+  </si>
+  <si>
+    <t>NSW_19</t>
+  </si>
+  <si>
+    <t>NSW_20</t>
+  </si>
+  <si>
+    <t>NSW_21</t>
+  </si>
+  <si>
+    <t>NSW_22</t>
+  </si>
+  <si>
+    <t>NSW_23</t>
+  </si>
+  <si>
+    <t>NSW_24</t>
+  </si>
+  <si>
+    <t>NSW_25</t>
+  </si>
+  <si>
+    <t>NSW_26</t>
+  </si>
+  <si>
+    <t>NSW_27</t>
+  </si>
+  <si>
+    <t>NSW_28</t>
+  </si>
+  <si>
+    <t>NSW_29</t>
+  </si>
+  <si>
+    <t>-33.8736</t>
+  </si>
+  <si>
+    <t>-33.8170</t>
+  </si>
+  <si>
+    <t>-33.7510</t>
+  </si>
+  <si>
+    <t>-33.7117</t>
+  </si>
+  <si>
+    <t>-33.4844</t>
+  </si>
+  <si>
+    <t>-33.4191</t>
+  </si>
+  <si>
+    <t>-33.5284</t>
+  </si>
+  <si>
+    <t>-33.2833</t>
+  </si>
+  <si>
+    <t>-33.1378</t>
+  </si>
+  <si>
+    <t>-33.0885</t>
+  </si>
+  <si>
+    <t>-32.9115</t>
+  </si>
+  <si>
+    <t>-32.8975</t>
+  </si>
+  <si>
+    <t>-32.8447</t>
+  </si>
+  <si>
+    <t>-32.3980</t>
+  </si>
+  <si>
+    <t>-31.9535</t>
+  </si>
+  <si>
+    <t>Blue Mountains</t>
+  </si>
+  <si>
+    <t>Central West</t>
+  </si>
+  <si>
+    <t>Far West</t>
   </si>
 </sst>
 </file>
@@ -639,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A3C533-154F-42EF-A106-DD2085AC4224}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -954,104 +1200,584 @@
         <v>146.91999999999999</v>
       </c>
     </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F18">
+        <v>151.09440000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F19">
+        <v>151.00299999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F20">
+        <v>150.69499999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
+        <v>154</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F21">
+        <v>150.31110000000001</v>
+      </c>
+    </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>128</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>113</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
+        <v>155</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>70</v>
+        <v>143</v>
       </c>
       <c r="F22">
-        <v>144.95249999999999</v>
+        <v>150.15360000000001</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>114</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" t="s">
-        <v>69</v>
+        <v>155</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>71</v>
+        <v>144</v>
       </c>
       <c r="F23">
-        <v>144.91829999999999</v>
+        <v>149.5771</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>130</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>115</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
+        <v>155</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="F24">
-        <v>145.1344</v>
+        <v>149.24719999999999</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>131</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>116</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>155</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>73</v>
+        <v>146</v>
       </c>
       <c r="F25">
-        <v>145.9836</v>
+        <v>149.1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" t="s">
+        <v>155</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F26">
+        <v>148.17500000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" t="s">
+        <v>155</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F27">
+        <v>147.15270000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>134</v>
+      </c>
+      <c r="B28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" t="s">
+        <v>156</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F28">
+        <v>146.64619999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" t="s">
+        <v>156</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F29">
+        <v>144.30199999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" t="s">
+        <v>156</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F30">
+        <v>143.37970000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>137</v>
+      </c>
+      <c r="B31" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" t="s">
+        <v>156</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F31">
+        <v>142.41900000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B32" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" t="s">
+        <v>156</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F32">
+        <v>141.45349999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F35">
+        <v>144.95249999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
+        <v>45</v>
+      </c>
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36">
+        <v>144.91829999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F37">
+        <v>145.1344</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" t="s">
+        <v>45</v>
+      </c>
+      <c r="D38" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38">
+        <v>145.9836</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>43</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B39" t="s">
         <v>34</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C39" t="s">
         <v>45</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D39" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F26">
+      <c r="F39">
         <v>146.3252</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" t="s">
+        <v>95</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F40">
+        <v>144.35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" t="s">
+        <v>96</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F41">
+        <v>142.93270000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F42">
+        <v>142.77860000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" t="s">
+        <v>94</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F43">
+        <v>142.19909999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" t="s">
+        <v>94</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F44">
+        <v>142.03120000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45" t="s">
+        <v>94</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F45">
+        <v>141.65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" t="s">
+        <v>105</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F50">
+        <v>138.5686</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" t="s">
+        <v>93</v>
+      </c>
+      <c r="D51" t="s">
+        <v>104</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F51">
+        <v>139.273</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" t="s">
+        <v>91</v>
+      </c>
+      <c r="C52" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" t="s">
+        <v>103</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F52">
+        <v>140.77000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>